<commit_message>
updated lit review counts
</commit_message>
<xml_diff>
--- a/Lit review data/cleaned lit review results.xlsx
+++ b/Lit review data/cleaned lit review results.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/catherineschluth/bansallab/humanhelminths/Lit review data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CAAD0B55-F620-794A-908C-6E005E14FC41}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1F368707-FC0A-2D4B-A575-242DA7230ED6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="320" yWindow="460" windowWidth="28260" windowHeight="16420" xr2:uid="{6572F45F-1008-5345-97C2-68802297C706}"/>
+    <workbookView xWindow="4900" yWindow="460" windowWidth="28260" windowHeight="16420" xr2:uid="{6572F45F-1008-5345-97C2-68802297C706}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1239,15 +1239,15 @@
         <v>244</v>
       </c>
       <c r="D2">
-        <f>SUM(B2, C2)</f>
+        <f t="shared" ref="D2:D65" si="0">SUM(B2, C2)</f>
         <v>2706</v>
       </c>
       <c r="E2">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="F2">
-        <f>(D2-E2)</f>
-        <v>2605</v>
+        <f t="shared" ref="F2:F65" si="1">(D2-E2)</f>
+        <v>2618</v>
       </c>
       <c r="G2">
         <v>197</v>
@@ -1264,15 +1264,15 @@
         <v>76</v>
       </c>
       <c r="D3">
-        <f>SUM(B3, C3)</f>
+        <f t="shared" si="0"/>
         <v>801</v>
       </c>
       <c r="E3">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="F3">
-        <f>(D3-E3)</f>
-        <v>716</v>
+        <f t="shared" si="1"/>
+        <v>726</v>
       </c>
       <c r="G3">
         <v>114</v>
@@ -1289,15 +1289,15 @@
         <v>57</v>
       </c>
       <c r="D4">
-        <f>SUM(B4, C4)</f>
+        <f t="shared" si="0"/>
         <v>823</v>
       </c>
       <c r="E4">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="F4">
-        <f>(D4-E4)</f>
-        <v>749</v>
+        <f t="shared" si="1"/>
+        <v>756</v>
       </c>
       <c r="G4">
         <v>159</v>
@@ -1314,15 +1314,15 @@
         <v>59</v>
       </c>
       <c r="D5">
-        <f>SUM(B5, C5)</f>
+        <f t="shared" si="0"/>
         <v>746</v>
       </c>
       <c r="E5">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F5">
-        <f>(D5-E5)</f>
-        <v>700</v>
+        <f t="shared" si="1"/>
+        <v>701</v>
       </c>
       <c r="G5">
         <v>313</v>
@@ -1339,15 +1339,15 @@
         <v>36</v>
       </c>
       <c r="D6">
-        <f>SUM(B6, C6)</f>
+        <f t="shared" si="0"/>
         <v>476</v>
       </c>
       <c r="E6">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F6">
-        <f>(D6-E6)</f>
-        <v>431</v>
+        <f t="shared" si="1"/>
+        <v>432</v>
       </c>
       <c r="G6">
         <v>244</v>
@@ -1364,15 +1364,15 @@
         <v>44</v>
       </c>
       <c r="D7">
-        <f>SUM(B7, C7)</f>
+        <f t="shared" si="0"/>
         <v>697</v>
       </c>
       <c r="E7">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F7">
-        <f>(D7-E7)</f>
-        <v>657</v>
+        <f t="shared" si="1"/>
+        <v>660</v>
       </c>
       <c r="G7">
         <v>141</v>
@@ -1389,15 +1389,15 @@
         <v>81</v>
       </c>
       <c r="D8">
-        <f>SUM(B8, C8)</f>
+        <f t="shared" si="0"/>
         <v>1085</v>
       </c>
       <c r="E8">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F8">
-        <f>(D8-E8)</f>
-        <v>1045</v>
+        <f t="shared" si="1"/>
+        <v>1047</v>
       </c>
       <c r="G8">
         <v>61</v>
@@ -1414,15 +1414,15 @@
         <v>59</v>
       </c>
       <c r="D9">
-        <f>SUM(B9, C9)</f>
+        <f t="shared" si="0"/>
         <v>503</v>
       </c>
       <c r="E9">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F9">
-        <f>(D9-E9)</f>
-        <v>466</v>
+        <f t="shared" si="1"/>
+        <v>467</v>
       </c>
       <c r="G9">
         <v>76</v>
@@ -1439,15 +1439,15 @@
         <v>30</v>
       </c>
       <c r="D10">
-        <f>SUM(B10, C10)</f>
+        <f t="shared" si="0"/>
         <v>456</v>
       </c>
       <c r="E10">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F10">
-        <f>(D10-E10)</f>
-        <v>435</v>
+        <f t="shared" si="1"/>
+        <v>438</v>
       </c>
       <c r="G10">
         <v>34</v>
@@ -1464,15 +1464,15 @@
         <v>38</v>
       </c>
       <c r="D11">
-        <f>SUM(B11, C11)</f>
+        <f t="shared" si="0"/>
         <v>310</v>
       </c>
       <c r="E11">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F11">
-        <f>(D11-E11)</f>
-        <v>292</v>
+        <f t="shared" si="1"/>
+        <v>293</v>
       </c>
       <c r="G11" s="3">
         <v>139</v>
@@ -1492,15 +1492,15 @@
         <v>18</v>
       </c>
       <c r="D12">
-        <f>SUM(B12, C12)</f>
+        <f t="shared" si="0"/>
         <v>347</v>
       </c>
       <c r="E12">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F12">
-        <f>(D12-E12)</f>
-        <v>333</v>
+        <f t="shared" si="1"/>
+        <v>334</v>
       </c>
       <c r="G12">
         <v>33</v>
@@ -1517,14 +1517,14 @@
         <v>19</v>
       </c>
       <c r="D13">
-        <f>SUM(B13, C13)</f>
+        <f t="shared" si="0"/>
         <v>245</v>
       </c>
       <c r="E13">
         <v>14</v>
       </c>
       <c r="F13">
-        <f>(D13-E13)</f>
+        <f t="shared" si="1"/>
         <v>231</v>
       </c>
       <c r="G13">
@@ -1542,14 +1542,14 @@
         <v>33</v>
       </c>
       <c r="D14">
-        <f>SUM(B14, C14)</f>
+        <f t="shared" si="0"/>
         <v>316</v>
       </c>
       <c r="E14">
         <v>10</v>
       </c>
       <c r="F14">
-        <f>(D14-E14)</f>
+        <f t="shared" si="1"/>
         <v>306</v>
       </c>
       <c r="G14" s="3">
@@ -1570,15 +1570,15 @@
         <v>14</v>
       </c>
       <c r="D15">
-        <f>SUM(B15, C15)</f>
+        <f t="shared" si="0"/>
         <v>202</v>
       </c>
       <c r="E15">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F15">
-        <f>(D15-E15)</f>
-        <v>192</v>
+        <f t="shared" si="1"/>
+        <v>193</v>
       </c>
       <c r="G15">
         <v>51</v>
@@ -1595,14 +1595,14 @@
         <v>10</v>
       </c>
       <c r="D16">
-        <f>SUM(B16, C16)</f>
+        <f t="shared" si="0"/>
         <v>97</v>
       </c>
       <c r="E16">
         <v>8</v>
       </c>
       <c r="F16">
-        <f>(D16-E16)</f>
+        <f t="shared" si="1"/>
         <v>89</v>
       </c>
       <c r="G16" s="3">
@@ -1623,15 +1623,15 @@
         <v>2</v>
       </c>
       <c r="D17">
-        <f>SUM(B17, C17)</f>
+        <f t="shared" si="0"/>
         <v>39</v>
       </c>
       <c r="E17">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F17">
-        <f>(D17-E17)</f>
-        <v>31</v>
+        <f t="shared" si="1"/>
+        <v>32</v>
       </c>
       <c r="G17">
         <v>57</v>
@@ -1648,15 +1648,15 @@
         <v>7</v>
       </c>
       <c r="D18">
-        <f>SUM(B18, C18)</f>
+        <f t="shared" si="0"/>
         <v>407</v>
       </c>
       <c r="E18">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F18">
-        <f>(D18-E18)</f>
-        <v>400</v>
+        <f t="shared" si="1"/>
+        <v>401</v>
       </c>
       <c r="G18">
         <v>85</v>
@@ -1673,15 +1673,15 @@
         <v>1</v>
       </c>
       <c r="D19">
-        <f>SUM(B19, C19)</f>
+        <f t="shared" si="0"/>
         <v>35</v>
       </c>
       <c r="E19">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F19">
-        <f>(D19-E19)</f>
-        <v>29</v>
+        <f t="shared" si="1"/>
+        <v>30</v>
       </c>
       <c r="G19">
         <v>33</v>
@@ -1698,14 +1698,14 @@
         <v>7</v>
       </c>
       <c r="D20">
-        <f>SUM(B20, C20)</f>
+        <f t="shared" si="0"/>
         <v>141</v>
       </c>
       <c r="E20">
         <v>5</v>
       </c>
       <c r="F20">
-        <f>(D20-E20)</f>
+        <f t="shared" si="1"/>
         <v>136</v>
       </c>
       <c r="G20">
@@ -1723,15 +1723,15 @@
         <v>8</v>
       </c>
       <c r="D21">
-        <f>SUM(B21, C21)</f>
+        <f t="shared" si="0"/>
         <v>112</v>
       </c>
       <c r="E21">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F21">
-        <f>(D21-E21)</f>
-        <v>107</v>
+        <f t="shared" si="1"/>
+        <v>108</v>
       </c>
       <c r="G21">
         <v>21</v>
@@ -1748,15 +1748,15 @@
         <v>1</v>
       </c>
       <c r="D22">
-        <f>SUM(B22, C22)</f>
+        <f t="shared" si="0"/>
         <v>35</v>
       </c>
       <c r="E22">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F22">
-        <f>(D22-E22)</f>
-        <v>30</v>
+        <f t="shared" si="1"/>
+        <v>33</v>
       </c>
       <c r="G22">
         <v>35</v>
@@ -1773,14 +1773,14 @@
         <v>58</v>
       </c>
       <c r="D23">
-        <f>SUM(B23, C23)</f>
+        <f t="shared" si="0"/>
         <v>1101</v>
       </c>
       <c r="E23">
         <v>4</v>
       </c>
       <c r="F23">
-        <f>(D23-E23)</f>
+        <f t="shared" si="1"/>
         <v>1097</v>
       </c>
       <c r="G23">
@@ -1798,15 +1798,15 @@
         <v>0</v>
       </c>
       <c r="D24">
-        <f>SUM(B24, C24)</f>
+        <f t="shared" si="0"/>
         <v>35</v>
       </c>
       <c r="E24">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F24">
-        <f>(D24-E24)</f>
-        <v>31</v>
+        <f t="shared" si="1"/>
+        <v>33</v>
       </c>
       <c r="G24">
         <v>9</v>
@@ -1823,14 +1823,14 @@
         <v>11</v>
       </c>
       <c r="D25">
-        <f>SUM(B25, C25)</f>
+        <f t="shared" si="0"/>
         <v>307</v>
       </c>
       <c r="E25">
         <v>3</v>
       </c>
       <c r="F25">
-        <f>(D25-E25)</f>
+        <f t="shared" si="1"/>
         <v>304</v>
       </c>
       <c r="G25" s="3">
@@ -1851,14 +1851,14 @@
         <v>10</v>
       </c>
       <c r="D26">
-        <f>SUM(B26, C26)</f>
+        <f t="shared" si="0"/>
         <v>259</v>
       </c>
       <c r="E26">
         <v>3</v>
       </c>
       <c r="F26">
-        <f>(D26-E26)</f>
+        <f t="shared" si="1"/>
         <v>256</v>
       </c>
       <c r="G26" s="3">
@@ -1879,14 +1879,14 @@
         <v>3</v>
       </c>
       <c r="D27">
-        <f>SUM(B27, C27)</f>
+        <f t="shared" si="0"/>
         <v>93</v>
       </c>
       <c r="E27">
         <v>3</v>
       </c>
       <c r="F27">
-        <f>(D27-E27)</f>
+        <f t="shared" si="1"/>
         <v>90</v>
       </c>
       <c r="G27">
@@ -1904,14 +1904,14 @@
         <v>2</v>
       </c>
       <c r="D28">
-        <f>SUM(B28, C28)</f>
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="E28">
         <v>3</v>
       </c>
       <c r="F28">
-        <f>(D28-E28)</f>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="G28">
@@ -1929,14 +1929,14 @@
         <v>0</v>
       </c>
       <c r="D29">
-        <f>SUM(B29, C29)</f>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="E29">
         <v>3</v>
       </c>
       <c r="F29">
-        <f>(D29-E29)</f>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="G29">
@@ -1954,14 +1954,14 @@
         <v>0</v>
       </c>
       <c r="D30">
-        <f>SUM(B30, C30)</f>
+        <f t="shared" si="0"/>
         <v>60</v>
       </c>
       <c r="E30">
         <v>2</v>
       </c>
       <c r="F30">
-        <f>(D30-E30)</f>
+        <f t="shared" si="1"/>
         <v>58</v>
       </c>
       <c r="G30" s="3">
@@ -1982,14 +1982,14 @@
         <v>4</v>
       </c>
       <c r="D31">
-        <f>SUM(B31, C31)</f>
+        <f t="shared" si="0"/>
         <v>42</v>
       </c>
       <c r="E31">
         <v>2</v>
       </c>
       <c r="F31">
-        <f>(D31-E31)</f>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="G31" s="1">
@@ -2007,14 +2007,14 @@
         <v>2</v>
       </c>
       <c r="D32">
-        <f>SUM(B32, C32)</f>
+        <f t="shared" si="0"/>
         <v>40</v>
       </c>
       <c r="E32">
         <v>2</v>
       </c>
       <c r="F32">
-        <f>(D32-E32)</f>
+        <f t="shared" si="1"/>
         <v>38</v>
       </c>
       <c r="G32" s="1">
@@ -2032,14 +2032,14 @@
         <v>2</v>
       </c>
       <c r="D33">
-        <f>SUM(B33, C33)</f>
+        <f t="shared" si="0"/>
         <v>38</v>
       </c>
       <c r="E33">
         <v>2</v>
       </c>
       <c r="F33">
-        <f>(D33-E33)</f>
+        <f t="shared" si="1"/>
         <v>36</v>
       </c>
       <c r="G33" s="1">
@@ -2057,14 +2057,14 @@
         <v>0</v>
       </c>
       <c r="D34">
-        <f>SUM(B34, C34)</f>
+        <f t="shared" si="0"/>
         <v>32</v>
       </c>
       <c r="E34">
         <v>2</v>
       </c>
       <c r="F34">
-        <f>(D34-E34)</f>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
       <c r="G34">
@@ -2082,15 +2082,15 @@
         <v>1</v>
       </c>
       <c r="D35">
-        <f>SUM(B35, C35)</f>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="E35">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F35">
-        <f>(D35-E35)</f>
-        <v>15</v>
+        <f t="shared" si="1"/>
+        <v>16</v>
       </c>
       <c r="G35">
         <v>13</v>
@@ -2107,14 +2107,14 @@
         <v>2</v>
       </c>
       <c r="D36">
-        <f>SUM(B36, C36)</f>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="E36">
         <v>2</v>
       </c>
       <c r="F36">
-        <f>(D36-E36)</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="G36">
@@ -2132,14 +2132,14 @@
         <v>5</v>
       </c>
       <c r="D37">
-        <f>SUM(B37, C37)</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="E37">
         <v>2</v>
       </c>
       <c r="F37">
-        <f>(D37-E37)</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="G37">
@@ -2157,15 +2157,15 @@
         <v>2</v>
       </c>
       <c r="D38">
-        <f>SUM(B38, C38)</f>
+        <f t="shared" si="0"/>
         <v>230</v>
       </c>
       <c r="E38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F38">
-        <f>(D38-E38)</f>
-        <v>229</v>
+        <f t="shared" si="1"/>
+        <v>230</v>
       </c>
       <c r="G38" s="1">
         <v>55</v>
@@ -2182,14 +2182,14 @@
         <v>5</v>
       </c>
       <c r="D39">
-        <f>SUM(B39, C39)</f>
+        <f t="shared" si="0"/>
         <v>65</v>
       </c>
       <c r="E39">
         <v>1</v>
       </c>
       <c r="F39">
-        <f>(D39-E39)</f>
+        <f t="shared" si="1"/>
         <v>64</v>
       </c>
       <c r="G39" s="3">
@@ -2210,14 +2210,14 @@
         <v>4</v>
       </c>
       <c r="D40">
-        <f>SUM(B40, C40)</f>
+        <f t="shared" si="0"/>
         <v>54</v>
       </c>
       <c r="E40">
         <v>1</v>
       </c>
       <c r="F40">
-        <f>(D40-E40)</f>
+        <f t="shared" si="1"/>
         <v>53</v>
       </c>
       <c r="G40" s="3">
@@ -2238,14 +2238,14 @@
         <v>0</v>
       </c>
       <c r="D41">
-        <f>SUM(B41, C41)</f>
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="E41">
         <v>1</v>
       </c>
       <c r="F41">
-        <f>(D41-E41)</f>
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
       <c r="G41" s="3">
@@ -2266,14 +2266,14 @@
         <v>0</v>
       </c>
       <c r="D42">
-        <f>SUM(B42, C42)</f>
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="E42">
         <v>1</v>
       </c>
       <c r="F42">
-        <f>(D42-E42)</f>
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
       <c r="G42">
@@ -2291,14 +2291,14 @@
         <v>2</v>
       </c>
       <c r="D43">
-        <f>SUM(B43, C43)</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="E43">
         <v>1</v>
       </c>
       <c r="F43">
-        <f>(D43-E43)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="G43">
@@ -2316,14 +2316,14 @@
         <v>1</v>
       </c>
       <c r="D44">
-        <f>SUM(B44, C44)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="E44">
         <v>1</v>
       </c>
       <c r="F44">
-        <f>(D44-E44)</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="G44" s="3">
@@ -2344,14 +2344,14 @@
         <v>0</v>
       </c>
       <c r="D45">
-        <f>SUM(B45, C45)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="E45">
         <v>1</v>
       </c>
       <c r="F45">
-        <f>(D45-E45)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="G45">
@@ -2369,14 +2369,14 @@
         <v>0</v>
       </c>
       <c r="D46">
-        <f>SUM(B46, C46)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="E46">
         <v>1</v>
       </c>
       <c r="F46">
-        <f>(D46-E46)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="G46">
@@ -2394,14 +2394,14 @@
         <v>2</v>
       </c>
       <c r="D47">
-        <f>SUM(B47, C47)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="E47">
         <v>1</v>
       </c>
       <c r="F47">
-        <f>(D47-E47)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="G47">
@@ -2419,14 +2419,14 @@
         <v>6</v>
       </c>
       <c r="D48">
-        <f>SUM(B48, C48)</f>
+        <f t="shared" si="0"/>
         <v>198</v>
       </c>
       <c r="E48">
         <v>0</v>
       </c>
       <c r="F48">
-        <f>(D48-E48)</f>
+        <f t="shared" si="1"/>
         <v>198</v>
       </c>
       <c r="G48">
@@ -2444,14 +2444,14 @@
         <v>1</v>
       </c>
       <c r="D49">
-        <f>SUM(B49, C49)</f>
+        <f t="shared" si="0"/>
         <v>169</v>
       </c>
       <c r="E49">
         <v>0</v>
       </c>
       <c r="F49">
-        <f>(D49-E49)</f>
+        <f t="shared" si="1"/>
         <v>169</v>
       </c>
       <c r="G49" s="3">
@@ -2472,14 +2472,14 @@
         <v>2</v>
       </c>
       <c r="D50">
-        <f>SUM(B50, C50)</f>
+        <f t="shared" si="0"/>
         <v>116</v>
       </c>
       <c r="E50">
         <v>0</v>
       </c>
       <c r="F50">
-        <f>(D50-E50)</f>
+        <f t="shared" si="1"/>
         <v>116</v>
       </c>
       <c r="G50">
@@ -2497,14 +2497,14 @@
         <v>0</v>
       </c>
       <c r="D51">
-        <f>SUM(B51, C51)</f>
+        <f t="shared" si="0"/>
         <v>116</v>
       </c>
       <c r="E51">
         <v>0</v>
       </c>
       <c r="F51">
-        <f>(D51-E51)</f>
+        <f t="shared" si="1"/>
         <v>116</v>
       </c>
       <c r="G51">
@@ -2522,14 +2522,14 @@
         <v>7</v>
       </c>
       <c r="D52">
-        <f>SUM(B52, C52)</f>
+        <f t="shared" si="0"/>
         <v>97</v>
       </c>
       <c r="E52">
         <v>0</v>
       </c>
       <c r="F52">
-        <f>(D52-E52)</f>
+        <f t="shared" si="1"/>
         <v>97</v>
       </c>
       <c r="G52">
@@ -2547,14 +2547,14 @@
         <v>1</v>
       </c>
       <c r="D53">
-        <f>SUM(B53, C53)</f>
+        <f t="shared" si="0"/>
         <v>69</v>
       </c>
       <c r="E53">
         <v>0</v>
       </c>
       <c r="F53">
-        <f>(D53-E53)</f>
+        <f t="shared" si="1"/>
         <v>69</v>
       </c>
       <c r="G53" s="3">
@@ -2575,14 +2575,14 @@
         <v>4</v>
       </c>
       <c r="D54">
-        <f>SUM(B54, C54)</f>
+        <f t="shared" si="0"/>
         <v>67</v>
       </c>
       <c r="E54">
         <v>0</v>
       </c>
       <c r="F54">
-        <f>(D54-E54)</f>
+        <f t="shared" si="1"/>
         <v>67</v>
       </c>
       <c r="G54">
@@ -2600,14 +2600,14 @@
         <v>12</v>
       </c>
       <c r="D55">
-        <f>SUM(B55, C55)</f>
+        <f t="shared" si="0"/>
         <v>66</v>
       </c>
       <c r="E55">
         <v>0</v>
       </c>
       <c r="F55">
-        <f>(D55-E55)</f>
+        <f t="shared" si="1"/>
         <v>66</v>
       </c>
       <c r="G55" s="3">
@@ -2628,14 +2628,14 @@
         <v>0</v>
       </c>
       <c r="D56">
-        <f>SUM(B56, C56)</f>
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="E56">
         <v>0</v>
       </c>
       <c r="F56">
-        <f>(D56-E56)</f>
+        <f t="shared" si="1"/>
         <v>22</v>
       </c>
       <c r="G56">
@@ -2653,14 +2653,14 @@
         <v>1</v>
       </c>
       <c r="D57">
-        <f>SUM(B57, C57)</f>
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="E57">
         <v>0</v>
       </c>
       <c r="F57">
-        <f>(D57-E57)</f>
+        <f t="shared" si="1"/>
         <v>22</v>
       </c>
       <c r="G57">
@@ -2678,14 +2678,14 @@
         <v>1</v>
       </c>
       <c r="D58">
-        <f>SUM(B58, C58)</f>
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="E58">
         <v>0</v>
       </c>
       <c r="F58">
-        <f>(D58-E58)</f>
+        <f t="shared" si="1"/>
         <v>22</v>
       </c>
       <c r="G58">
@@ -2703,14 +2703,14 @@
         <v>3</v>
       </c>
       <c r="D59">
-        <f>SUM(B59, C59)</f>
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="E59">
         <v>0</v>
       </c>
       <c r="F59">
-        <f>(D59-E59)</f>
+        <f t="shared" si="1"/>
         <v>23</v>
       </c>
       <c r="G59">
@@ -2728,14 +2728,14 @@
         <v>0</v>
       </c>
       <c r="D60">
-        <f>SUM(B60, C60)</f>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="E60">
         <v>0</v>
       </c>
       <c r="F60">
-        <f>(D60-E60)</f>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="G60">
@@ -2753,14 +2753,14 @@
         <v>3</v>
       </c>
       <c r="D61">
-        <f>SUM(B61, C61)</f>
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="E61">
         <v>0</v>
       </c>
       <c r="F61">
-        <f>(D61-E61)</f>
+        <f t="shared" si="1"/>
         <v>22</v>
       </c>
       <c r="G61">
@@ -2778,14 +2778,14 @@
         <v>1</v>
       </c>
       <c r="D62">
-        <f>SUM(B62, C62)</f>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="E62">
         <v>0</v>
       </c>
       <c r="F62">
-        <f>(D62-E62)</f>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="G62">
@@ -2803,14 +2803,14 @@
         <v>0</v>
       </c>
       <c r="D63">
-        <f>SUM(B63, C63)</f>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="E63">
         <v>0</v>
       </c>
       <c r="F63">
-        <f>(D63-E63)</f>
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="G63">
@@ -2828,14 +2828,14 @@
         <v>0</v>
       </c>
       <c r="D64">
-        <f>SUM(B64, C64)</f>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="E64">
         <v>0</v>
       </c>
       <c r="F64">
-        <f>(D64-E64)</f>
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="G64">
@@ -2853,14 +2853,14 @@
         <v>0</v>
       </c>
       <c r="D65">
-        <f>SUM(B65, C65)</f>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="E65">
         <v>0</v>
       </c>
       <c r="F65">
-        <f>(D65-E65)</f>
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="G65">
@@ -2878,14 +2878,14 @@
         <v>1</v>
       </c>
       <c r="D66">
-        <f>SUM(B66, C66)</f>
+        <f t="shared" ref="D66:D129" si="2">SUM(B66, C66)</f>
         <v>17</v>
       </c>
       <c r="E66">
         <v>0</v>
       </c>
       <c r="F66">
-        <f>(D66-E66)</f>
+        <f t="shared" ref="F66:F129" si="3">(D66-E66)</f>
         <v>17</v>
       </c>
       <c r="G66" s="3">
@@ -2906,14 +2906,14 @@
         <v>1</v>
       </c>
       <c r="D67">
-        <f>SUM(B67, C67)</f>
+        <f t="shared" si="2"/>
         <v>17</v>
       </c>
       <c r="E67">
         <v>0</v>
       </c>
       <c r="F67">
-        <f>(D67-E67)</f>
+        <f t="shared" si="3"/>
         <v>17</v>
       </c>
       <c r="G67">
@@ -2931,14 +2931,14 @@
         <v>0</v>
       </c>
       <c r="D68">
-        <f>SUM(B68, C68)</f>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="E68">
         <v>0</v>
       </c>
       <c r="F68">
-        <f>(D68-E68)</f>
+        <f t="shared" si="3"/>
         <v>14</v>
       </c>
       <c r="G68">
@@ -2956,14 +2956,14 @@
         <v>0</v>
       </c>
       <c r="D69">
-        <f>SUM(B69, C69)</f>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="E69">
         <v>0</v>
       </c>
       <c r="F69">
-        <f>(D69-E69)</f>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="G69">
@@ -2981,14 +2981,14 @@
         <v>0</v>
       </c>
       <c r="D70">
-        <f>SUM(B70, C70)</f>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="E70">
         <v>0</v>
       </c>
       <c r="F70">
-        <f>(D70-E70)</f>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="G70">
@@ -3006,14 +3006,14 @@
         <v>0</v>
       </c>
       <c r="D71">
-        <f>SUM(B71, C71)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="E71">
         <v>0</v>
       </c>
       <c r="F71">
-        <f>(D71-E71)</f>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="G71" s="3">
@@ -3034,14 +3034,14 @@
         <v>0</v>
       </c>
       <c r="D72">
-        <f>SUM(B72, C72)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="E72">
         <v>0</v>
       </c>
       <c r="F72">
-        <f>(D72-E72)</f>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="G72">
@@ -3059,14 +3059,14 @@
         <v>0</v>
       </c>
       <c r="D73">
-        <f>SUM(B73, C73)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="E73">
         <v>0</v>
       </c>
       <c r="F73">
-        <f>(D73-E73)</f>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="G73">
@@ -3084,14 +3084,14 @@
         <v>0</v>
       </c>
       <c r="D74">
-        <f>SUM(B74, C74)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="E74">
         <v>0</v>
       </c>
       <c r="F74">
-        <f>(D74-E74)</f>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="G74" s="3">
@@ -3112,14 +3112,14 @@
         <v>0</v>
       </c>
       <c r="D75">
-        <f>SUM(B75, C75)</f>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="E75">
         <v>0</v>
       </c>
       <c r="F75">
-        <f>(D75-E75)</f>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="G75" s="3">
@@ -3140,14 +3140,14 @@
         <v>0</v>
       </c>
       <c r="D76">
-        <f>SUM(B76, C76)</f>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="E76">
         <v>0</v>
       </c>
       <c r="F76">
-        <f>(D76-E76)</f>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="G76">
@@ -3165,14 +3165,14 @@
         <v>0</v>
       </c>
       <c r="D77">
-        <f>SUM(B77, C77)</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="E77">
         <v>0</v>
       </c>
       <c r="F77">
-        <f>(D77-E77)</f>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="G77">
@@ -3190,14 +3190,14 @@
         <v>0</v>
       </c>
       <c r="D78">
-        <f>SUM(B78, C78)</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="E78">
         <v>0</v>
       </c>
       <c r="F78">
-        <f>(D78-E78)</f>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="G78">
@@ -3215,14 +3215,14 @@
         <v>0</v>
       </c>
       <c r="D79">
-        <f>SUM(B79, C79)</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="E79">
         <v>0</v>
       </c>
       <c r="F79">
-        <f>(D79-E79)</f>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="G79" s="3">
@@ -3243,14 +3243,14 @@
         <v>0</v>
       </c>
       <c r="D80">
-        <f>SUM(B80, C80)</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="E80">
         <v>0</v>
       </c>
       <c r="F80">
-        <f>(D80-E80)</f>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="G80" s="3">
@@ -3271,14 +3271,14 @@
         <v>0</v>
       </c>
       <c r="D81">
-        <f>SUM(B81, C81)</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="E81">
         <v>0</v>
       </c>
       <c r="F81">
-        <f>(D81-E81)</f>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="G81">
@@ -3296,14 +3296,14 @@
         <v>1</v>
       </c>
       <c r="D82">
-        <f>SUM(B82, C82)</f>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="E82">
         <v>0</v>
       </c>
       <c r="F82">
-        <f>(D82-E82)</f>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="G82">
@@ -3321,14 +3321,14 @@
         <v>0</v>
       </c>
       <c r="D83">
-        <f>SUM(B83, C83)</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="E83">
         <v>0</v>
       </c>
       <c r="F83">
-        <f>(D83-E83)</f>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="G83">
@@ -3346,14 +3346,14 @@
         <v>0</v>
       </c>
       <c r="D84">
-        <f>SUM(B84, C84)</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="E84">
         <v>0</v>
       </c>
       <c r="F84">
-        <f>(D84-E84)</f>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="G84">
@@ -3371,14 +3371,14 @@
         <v>0</v>
       </c>
       <c r="D85">
-        <f>SUM(B85, C85)</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="E85">
         <v>0</v>
       </c>
       <c r="F85">
-        <f>(D85-E85)</f>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="G85">
@@ -3396,14 +3396,14 @@
         <v>1</v>
       </c>
       <c r="D86">
-        <f>SUM(B86, C86)</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="E86">
         <v>0</v>
       </c>
       <c r="F86">
-        <f>(D86-E86)</f>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="G86">
@@ -3421,14 +3421,14 @@
         <v>1</v>
       </c>
       <c r="D87">
-        <f>SUM(B87, C87)</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="E87">
         <v>0</v>
       </c>
       <c r="F87">
-        <f>(D87-E87)</f>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="G87">
@@ -3446,14 +3446,14 @@
         <v>0</v>
       </c>
       <c r="D88">
-        <f>SUM(B88, C88)</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="E88">
         <v>0</v>
       </c>
       <c r="F88">
-        <f>(D88-E88)</f>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="G88">
@@ -3471,14 +3471,14 @@
         <v>0</v>
       </c>
       <c r="D89">
-        <f>SUM(B89, C89)</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="E89">
         <v>0</v>
       </c>
       <c r="F89">
-        <f>(D89-E89)</f>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="G89">
@@ -3496,14 +3496,14 @@
         <v>0</v>
       </c>
       <c r="D90">
-        <f>SUM(B90, C90)</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="E90">
         <v>0</v>
       </c>
       <c r="F90">
-        <f>(D90-E90)</f>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="G90">
@@ -3521,14 +3521,14 @@
         <v>0</v>
       </c>
       <c r="D91">
-        <f>SUM(B91, C91)</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="E91">
         <v>0</v>
       </c>
       <c r="F91">
-        <f>(D91-E91)</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="G91" s="3">
@@ -3549,14 +3549,14 @@
         <v>0</v>
       </c>
       <c r="D92">
-        <f>SUM(B92, C92)</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="E92">
         <v>0</v>
       </c>
       <c r="F92">
-        <f>(D92-E92)</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="G92">
@@ -3574,14 +3574,14 @@
         <v>0</v>
       </c>
       <c r="D93">
-        <f>SUM(B93, C93)</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="E93">
         <v>0</v>
       </c>
       <c r="F93">
-        <f>(D93-E93)</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="G93">
@@ -3599,14 +3599,14 @@
         <v>0</v>
       </c>
       <c r="D94">
-        <f>SUM(B94, C94)</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="E94">
         <v>0</v>
       </c>
       <c r="F94">
-        <f>(D94-E94)</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="G94">
@@ -3624,14 +3624,14 @@
         <v>0</v>
       </c>
       <c r="D95">
-        <f>SUM(B95, C95)</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="E95">
         <v>0</v>
       </c>
       <c r="F95">
-        <f>(D95-E95)</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="G95">
@@ -3649,14 +3649,14 @@
         <v>0</v>
       </c>
       <c r="D96">
-        <f>SUM(B96, C96)</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="E96">
         <v>0</v>
       </c>
       <c r="F96">
-        <f>(D96-E96)</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="G96">
@@ -3674,14 +3674,14 @@
         <v>0</v>
       </c>
       <c r="D97">
-        <f>SUM(B97, C97)</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="E97">
         <v>0</v>
       </c>
       <c r="F97">
-        <f>(D97-E97)</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="G97">
@@ -3699,14 +3699,14 @@
         <v>1</v>
       </c>
       <c r="D98">
-        <f>SUM(B98, C98)</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="E98">
         <v>0</v>
       </c>
       <c r="F98">
-        <f>(D98-E98)</f>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="G98" s="3">
@@ -3727,14 +3727,14 @@
         <v>0</v>
       </c>
       <c r="D99">
-        <f>SUM(B99, C99)</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="E99">
         <v>0</v>
       </c>
       <c r="F99">
-        <f>(D99-E99)</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="G99">
@@ -3752,14 +3752,14 @@
         <v>0</v>
       </c>
       <c r="D100">
-        <f>SUM(B100, C100)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="E100">
         <v>0</v>
       </c>
       <c r="F100">
-        <f>(D100-E100)</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="G100">
@@ -3777,14 +3777,14 @@
         <v>0</v>
       </c>
       <c r="D101">
-        <f>SUM(B101, C101)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="E101">
         <v>0</v>
       </c>
       <c r="F101">
-        <f>(D101-E101)</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="G101">
@@ -3802,14 +3802,14 @@
         <v>2</v>
       </c>
       <c r="D102">
-        <f>SUM(B102, C102)</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="E102">
         <v>0</v>
       </c>
       <c r="F102">
-        <f>(D102-E102)</f>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="G102" s="3">
@@ -3830,14 +3830,14 @@
         <v>3</v>
       </c>
       <c r="D103">
-        <f>SUM(B103, C103)</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="E103">
         <v>0</v>
       </c>
       <c r="F103">
-        <f>(D103-E103)</f>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="G103">
@@ -3855,14 +3855,14 @@
         <v>0</v>
       </c>
       <c r="D104">
-        <f>SUM(B104, C104)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="E104">
         <v>0</v>
       </c>
       <c r="F104">
-        <f>(D104-E104)</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="G104">
@@ -3880,14 +3880,14 @@
         <v>0</v>
       </c>
       <c r="D105">
-        <f>SUM(B105, C105)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="E105">
         <v>0</v>
       </c>
       <c r="F105">
-        <f>(D105-E105)</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="G105">
@@ -3905,14 +3905,14 @@
         <v>0</v>
       </c>
       <c r="D106">
-        <f>SUM(B106, C106)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="E106">
         <v>0</v>
       </c>
       <c r="F106">
-        <f>(D106-E106)</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="G106">
@@ -3930,14 +3930,14 @@
         <v>0</v>
       </c>
       <c r="D107">
-        <f>SUM(B107, C107)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="E107">
         <v>0</v>
       </c>
       <c r="F107">
-        <f>(D107-E107)</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="G107">
@@ -3955,14 +3955,14 @@
         <v>0</v>
       </c>
       <c r="D108">
-        <f>SUM(B108, C108)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="E108">
         <v>0</v>
       </c>
       <c r="F108">
-        <f>(D108-E108)</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="G108">
@@ -3980,14 +3980,14 @@
         <v>0</v>
       </c>
       <c r="D109">
-        <f>SUM(B109, C109)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="E109">
         <v>0</v>
       </c>
       <c r="F109">
-        <f>(D109-E109)</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="G109">
@@ -4005,14 +4005,14 @@
         <v>0</v>
       </c>
       <c r="D110">
-        <f>SUM(B110, C110)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="E110">
         <v>0</v>
       </c>
       <c r="F110">
-        <f>(D110-E110)</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="G110">
@@ -4030,14 +4030,14 @@
         <v>0</v>
       </c>
       <c r="D111">
-        <f>SUM(B111, C111)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="E111">
         <v>0</v>
       </c>
       <c r="F111">
-        <f>(D111-E111)</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="G111">
@@ -4055,14 +4055,14 @@
         <v>0</v>
       </c>
       <c r="D112">
-        <f>SUM(B112, C112)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="E112">
         <v>0</v>
       </c>
       <c r="F112">
-        <f>(D112-E112)</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="G112">
@@ -4080,14 +4080,14 @@
         <v>0</v>
       </c>
       <c r="D113">
-        <f>SUM(B113, C113)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="E113">
         <v>0</v>
       </c>
       <c r="F113">
-        <f>(D113-E113)</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="G113">
@@ -4105,14 +4105,14 @@
         <v>0</v>
       </c>
       <c r="D114">
-        <f>SUM(B114, C114)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="E114">
         <v>0</v>
       </c>
       <c r="F114">
-        <f>(D114-E114)</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="G114">
@@ -4130,14 +4130,14 @@
         <v>0</v>
       </c>
       <c r="D115">
-        <f>SUM(B115, C115)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="E115">
         <v>0</v>
       </c>
       <c r="F115">
-        <f>(D115-E115)</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="G115">
@@ -4155,14 +4155,14 @@
         <v>0</v>
       </c>
       <c r="D116">
-        <f>SUM(B116, C116)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="E116">
         <v>0</v>
       </c>
       <c r="F116">
-        <f>(D116-E116)</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="G116" s="3">
@@ -4183,14 +4183,14 @@
         <v>0</v>
       </c>
       <c r="D117">
-        <f>SUM(B117, C117)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="E117">
         <v>0</v>
       </c>
       <c r="F117">
-        <f>(D117-E117)</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="G117">
@@ -4208,14 +4208,14 @@
         <v>0</v>
       </c>
       <c r="D118">
-        <f>SUM(B118, C118)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="E118">
         <v>0</v>
       </c>
       <c r="F118">
-        <f>(D118-E118)</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="G118">
@@ -4233,14 +4233,14 @@
         <v>0</v>
       </c>
       <c r="D119">
-        <f>SUM(B119, C119)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="E119">
         <v>0</v>
       </c>
       <c r="F119">
-        <f>(D119-E119)</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="G119">
@@ -4258,14 +4258,14 @@
         <v>0</v>
       </c>
       <c r="D120">
-        <f>SUM(B120, C120)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="E120">
         <v>0</v>
       </c>
       <c r="F120">
-        <f>(D120-E120)</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="G120">
@@ -4283,14 +4283,14 @@
         <v>0</v>
       </c>
       <c r="D121">
-        <f>SUM(B121, C121)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="E121">
         <v>0</v>
       </c>
       <c r="F121">
-        <f>(D121-E121)</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="G121">
@@ -4308,14 +4308,14 @@
         <v>0</v>
       </c>
       <c r="D122">
-        <f>SUM(B122, C122)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="E122">
         <v>0</v>
       </c>
       <c r="F122">
-        <f>(D122-E122)</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="G122">
@@ -4333,14 +4333,14 @@
         <v>1</v>
       </c>
       <c r="D123">
-        <f>SUM(B123, C123)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="E123">
         <v>0</v>
       </c>
       <c r="F123">
-        <f>(D123-E123)</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="G123">
@@ -4358,14 +4358,14 @@
         <v>0</v>
       </c>
       <c r="D124">
-        <f>SUM(B124, C124)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="E124">
         <v>0</v>
       </c>
       <c r="F124">
-        <f>(D124-E124)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="G124">
@@ -4383,14 +4383,14 @@
         <v>0</v>
       </c>
       <c r="D125">
-        <f>SUM(B125, C125)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="E125">
         <v>0</v>
       </c>
       <c r="F125">
-        <f>(D125-E125)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="G125">
@@ -4408,14 +4408,14 @@
         <v>0</v>
       </c>
       <c r="D126">
-        <f>SUM(B126, C126)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="E126">
         <v>0</v>
       </c>
       <c r="F126">
-        <f>(D126-E126)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="G126">
@@ -4433,14 +4433,14 @@
         <v>0</v>
       </c>
       <c r="D127">
-        <f>SUM(B127, C127)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="E127">
         <v>0</v>
       </c>
       <c r="F127">
-        <f>(D127-E127)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="G127">
@@ -4458,14 +4458,14 @@
         <v>0</v>
       </c>
       <c r="D128">
-        <f>SUM(B128, C128)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="E128">
         <v>0</v>
       </c>
       <c r="F128">
-        <f>(D128-E128)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="G128">
@@ -4483,14 +4483,14 @@
         <v>0</v>
       </c>
       <c r="D129">
-        <f>SUM(B129, C129)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="E129">
         <v>0</v>
       </c>
       <c r="F129">
-        <f>(D129-E129)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="G129">
@@ -4508,14 +4508,14 @@
         <v>0</v>
       </c>
       <c r="D130">
-        <f>SUM(B130, C130)</f>
+        <f t="shared" ref="D130:D193" si="4">SUM(B130, C130)</f>
         <v>1</v>
       </c>
       <c r="E130">
         <v>0</v>
       </c>
       <c r="F130">
-        <f>(D130-E130)</f>
+        <f t="shared" ref="F130:F193" si="5">(D130-E130)</f>
         <v>1</v>
       </c>
       <c r="G130">
@@ -4533,14 +4533,14 @@
         <v>0</v>
       </c>
       <c r="D131">
-        <f>SUM(B131, C131)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="E131">
         <v>0</v>
       </c>
       <c r="F131">
-        <f>(D131-E131)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="G131">
@@ -4558,14 +4558,14 @@
         <v>0</v>
       </c>
       <c r="D132">
-        <f>SUM(B132, C132)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="E132">
         <v>0</v>
       </c>
       <c r="F132">
-        <f>(D132-E132)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="G132" s="3">
@@ -4586,14 +4586,14 @@
         <v>0</v>
       </c>
       <c r="D133">
-        <f>SUM(B133, C133)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="E133">
         <v>0</v>
       </c>
       <c r="F133">
-        <f>(D133-E133)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="G133">
@@ -4611,14 +4611,14 @@
         <v>0</v>
       </c>
       <c r="D134">
-        <f>SUM(B134, C134)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="E134">
         <v>0</v>
       </c>
       <c r="F134">
-        <f>(D134-E134)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="G134">
@@ -4636,14 +4636,14 @@
         <v>0</v>
       </c>
       <c r="D135">
-        <f>SUM(B135, C135)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="E135">
         <v>0</v>
       </c>
       <c r="F135">
-        <f>(D135-E135)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="G135">
@@ -4661,14 +4661,14 @@
         <v>0</v>
       </c>
       <c r="D136">
-        <f>SUM(B136, C136)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="E136">
         <v>0</v>
       </c>
       <c r="F136">
-        <f>(D136-E136)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="G136">
@@ -4686,14 +4686,14 @@
         <v>0</v>
       </c>
       <c r="D137">
-        <f>SUM(B137, C137)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="E137">
         <v>0</v>
       </c>
       <c r="F137">
-        <f>(D137-E137)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="G137">
@@ -4711,14 +4711,14 @@
         <v>0</v>
       </c>
       <c r="D138">
-        <f>SUM(B138, C138)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="E138">
         <v>0</v>
       </c>
       <c r="F138">
-        <f>(D138-E138)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="G138">
@@ -4736,14 +4736,14 @@
         <v>0</v>
       </c>
       <c r="D139">
-        <f>SUM(B139, C139)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="E139">
         <v>0</v>
       </c>
       <c r="F139">
-        <f>(D139-E139)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="G139">
@@ -4761,14 +4761,14 @@
         <v>0</v>
       </c>
       <c r="D140">
-        <f>SUM(B140, C140)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="E140">
         <v>0</v>
       </c>
       <c r="F140">
-        <f>(D140-E140)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="G140">
@@ -4786,14 +4786,14 @@
         <v>0</v>
       </c>
       <c r="D141">
-        <f>SUM(B141, C141)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="E141">
         <v>0</v>
       </c>
       <c r="F141">
-        <f>(D141-E141)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="G141">
@@ -4811,14 +4811,14 @@
         <v>0</v>
       </c>
       <c r="D142">
-        <f>SUM(B142, C142)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="E142">
         <v>0</v>
       </c>
       <c r="F142">
-        <f>(D142-E142)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="G142">
@@ -4836,14 +4836,14 @@
         <v>0</v>
       </c>
       <c r="D143">
-        <f>SUM(B143, C143)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="E143">
         <v>0</v>
       </c>
       <c r="F143">
-        <f>(D143-E143)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="G143">
@@ -4861,14 +4861,14 @@
         <v>0</v>
       </c>
       <c r="D144">
-        <f>SUM(B144, C144)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="E144">
         <v>0</v>
       </c>
       <c r="F144">
-        <f>(D144-E144)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="G144">
@@ -4886,14 +4886,14 @@
         <v>0</v>
       </c>
       <c r="D145">
-        <f>SUM(B145, C145)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="E145">
         <v>0</v>
       </c>
       <c r="F145">
-        <f>(D145-E145)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="G145">
@@ -4911,14 +4911,14 @@
         <v>0</v>
       </c>
       <c r="D146">
-        <f>SUM(B146, C146)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="E146">
         <v>0</v>
       </c>
       <c r="F146">
-        <f>(D146-E146)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="G146">
@@ -4936,14 +4936,14 @@
         <v>0</v>
       </c>
       <c r="D147">
-        <f>SUM(B147, C147)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="E147">
         <v>0</v>
       </c>
       <c r="F147">
-        <f>(D147-E147)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="G147">
@@ -4961,14 +4961,14 @@
         <v>0</v>
       </c>
       <c r="D148">
-        <f>SUM(B148, C148)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="E148">
         <v>0</v>
       </c>
       <c r="F148">
-        <f>(D148-E148)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="G148">
@@ -4986,14 +4986,14 @@
         <v>0</v>
       </c>
       <c r="D149">
-        <f>SUM(B149, C149)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="E149">
         <v>0</v>
       </c>
       <c r="F149">
-        <f>(D149-E149)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="G149">
@@ -5011,14 +5011,14 @@
         <v>0</v>
       </c>
       <c r="D150">
-        <f>SUM(B150, C150)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="E150">
         <v>0</v>
       </c>
       <c r="F150">
-        <f>(D150-E150)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="G150">
@@ -5036,14 +5036,14 @@
         <v>0</v>
       </c>
       <c r="D151">
-        <f>SUM(B151, C151)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E151">
         <v>0</v>
       </c>
       <c r="F151">
-        <f>(D151-E151)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G151">
@@ -5061,14 +5061,14 @@
         <v>0</v>
       </c>
       <c r="D152">
-        <f>SUM(B152, C152)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E152">
         <v>0</v>
       </c>
       <c r="F152">
-        <f>(D152-E152)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G152">
@@ -5086,14 +5086,14 @@
         <v>0</v>
       </c>
       <c r="D153">
-        <f>SUM(B153, C153)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E153">
         <v>0</v>
       </c>
       <c r="F153">
-        <f>(D153-E153)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G153">
@@ -5111,14 +5111,14 @@
         <v>0</v>
       </c>
       <c r="D154">
-        <f>SUM(B154, C154)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E154">
         <v>0</v>
       </c>
       <c r="F154">
-        <f>(D154-E154)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G154">
@@ -5136,14 +5136,14 @@
         <v>0</v>
       </c>
       <c r="D155">
-        <f>SUM(B155, C155)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E155">
         <v>0</v>
       </c>
       <c r="F155">
-        <f>(D155-E155)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G155">
@@ -5161,14 +5161,14 @@
         <v>0</v>
       </c>
       <c r="D156">
-        <f>SUM(B156, C156)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E156">
         <v>0</v>
       </c>
       <c r="F156">
-        <f>(D156-E156)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G156">
@@ -5186,14 +5186,14 @@
         <v>0</v>
       </c>
       <c r="D157">
-        <f>SUM(B157, C157)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E157">
         <v>0</v>
       </c>
       <c r="F157">
-        <f>(D157-E157)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G157">
@@ -5211,14 +5211,14 @@
         <v>0</v>
       </c>
       <c r="D158">
-        <f>SUM(B158, C158)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E158">
         <v>0</v>
       </c>
       <c r="F158">
-        <f>(D158-E158)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G158">
@@ -5236,14 +5236,14 @@
         <v>0</v>
       </c>
       <c r="D159">
-        <f>SUM(B159, C159)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E159">
         <v>0</v>
       </c>
       <c r="F159">
-        <f>(D159-E159)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G159">
@@ -5261,14 +5261,14 @@
         <v>0</v>
       </c>
       <c r="D160">
-        <f>SUM(B160, C160)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E160">
         <v>0</v>
       </c>
       <c r="F160">
-        <f>(D160-E160)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G160">
@@ -5286,14 +5286,14 @@
         <v>0</v>
       </c>
       <c r="D161">
-        <f>SUM(B161, C161)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E161">
         <v>0</v>
       </c>
       <c r="F161">
-        <f>(D161-E161)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G161">
@@ -5311,14 +5311,14 @@
         <v>0</v>
       </c>
       <c r="D162">
-        <f>SUM(B162, C162)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E162">
         <v>0</v>
       </c>
       <c r="F162">
-        <f>(D162-E162)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G162">
@@ -5336,14 +5336,14 @@
         <v>0</v>
       </c>
       <c r="D163">
-        <f>SUM(B163, C163)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E163">
         <v>0</v>
       </c>
       <c r="F163">
-        <f>(D163-E163)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G163">
@@ -5361,14 +5361,14 @@
         <v>0</v>
       </c>
       <c r="D164">
-        <f>SUM(B164, C164)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E164">
         <v>0</v>
       </c>
       <c r="F164">
-        <f>(D164-E164)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G164">
@@ -5386,14 +5386,14 @@
         <v>0</v>
       </c>
       <c r="D165">
-        <f>SUM(B165, C165)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E165">
         <v>0</v>
       </c>
       <c r="F165">
-        <f>(D165-E165)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G165">
@@ -5411,14 +5411,14 @@
         <v>0</v>
       </c>
       <c r="D166">
-        <f>SUM(B166, C166)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E166">
         <v>0</v>
       </c>
       <c r="F166">
-        <f>(D166-E166)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G166">
@@ -5436,14 +5436,14 @@
         <v>0</v>
       </c>
       <c r="D167">
-        <f>SUM(B167, C167)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E167">
         <v>0</v>
       </c>
       <c r="F167">
-        <f>(D167-E167)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G167">
@@ -5461,14 +5461,14 @@
         <v>0</v>
       </c>
       <c r="D168">
-        <f>SUM(B168, C168)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E168">
         <v>0</v>
       </c>
       <c r="F168">
-        <f>(D168-E168)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G168">
@@ -5486,14 +5486,14 @@
         <v>0</v>
       </c>
       <c r="D169">
-        <f>SUM(B169, C169)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E169">
         <v>0</v>
       </c>
       <c r="F169">
-        <f>(D169-E169)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G169">
@@ -5511,14 +5511,14 @@
         <v>0</v>
       </c>
       <c r="D170">
-        <f>SUM(B170, C170)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E170">
         <v>0</v>
       </c>
       <c r="F170">
-        <f>(D170-E170)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G170">
@@ -5536,14 +5536,14 @@
         <v>0</v>
       </c>
       <c r="D171">
-        <f>SUM(B171, C171)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E171">
         <v>0</v>
       </c>
       <c r="F171">
-        <f>(D171-E171)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G171">
@@ -5561,14 +5561,14 @@
         <v>0</v>
       </c>
       <c r="D172">
-        <f>SUM(B172, C172)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E172">
         <v>0</v>
       </c>
       <c r="F172">
-        <f>(D172-E172)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G172">
@@ -5586,14 +5586,14 @@
         <v>0</v>
       </c>
       <c r="D173">
-        <f>SUM(B173, C173)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E173">
         <v>0</v>
       </c>
       <c r="F173">
-        <f>(D173-E173)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G173">
@@ -5611,14 +5611,14 @@
         <v>0</v>
       </c>
       <c r="D174">
-        <f>SUM(B174, C174)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E174">
         <v>0</v>
       </c>
       <c r="F174">
-        <f>(D174-E174)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G174">
@@ -5636,14 +5636,14 @@
         <v>0</v>
       </c>
       <c r="D175">
-        <f>SUM(B175, C175)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E175">
         <v>0</v>
       </c>
       <c r="F175">
-        <f>(D175-E175)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G175">
@@ -5661,14 +5661,14 @@
         <v>0</v>
       </c>
       <c r="D176">
-        <f>SUM(B176, C176)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E176">
         <v>0</v>
       </c>
       <c r="F176">
-        <f>(D176-E176)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G176">
@@ -5686,14 +5686,14 @@
         <v>0</v>
       </c>
       <c r="D177">
-        <f>SUM(B177, C177)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E177">
         <v>0</v>
       </c>
       <c r="F177">
-        <f>(D177-E177)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G177">
@@ -5711,14 +5711,14 @@
         <v>0</v>
       </c>
       <c r="D178">
-        <f>SUM(B178, C178)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E178">
         <v>0</v>
       </c>
       <c r="F178">
-        <f>(D178-E178)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G178">
@@ -5736,14 +5736,14 @@
         <v>0</v>
       </c>
       <c r="D179">
-        <f>SUM(B179, C179)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E179">
         <v>0</v>
       </c>
       <c r="F179">
-        <f>(D179-E179)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G179">
@@ -5761,14 +5761,14 @@
         <v>0</v>
       </c>
       <c r="D180">
-        <f>SUM(B180, C180)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E180">
         <v>0</v>
       </c>
       <c r="F180">
-        <f>(D180-E180)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G180">
@@ -5786,14 +5786,14 @@
         <v>0</v>
       </c>
       <c r="D181">
-        <f>SUM(B181, C181)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E181">
         <v>0</v>
       </c>
       <c r="F181">
-        <f>(D181-E181)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G181" s="3">
@@ -5814,14 +5814,14 @@
         <v>0</v>
       </c>
       <c r="D182">
-        <f>SUM(B182, C182)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E182">
         <v>0</v>
       </c>
       <c r="F182">
-        <f>(D182-E182)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G182">
@@ -5839,14 +5839,14 @@
         <v>0</v>
       </c>
       <c r="D183">
-        <f>SUM(B183, C183)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E183">
         <v>0</v>
       </c>
       <c r="F183">
-        <f>(D183-E183)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G183" s="3">
@@ -5867,14 +5867,14 @@
         <v>0</v>
       </c>
       <c r="D184">
-        <f>SUM(B184, C184)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E184">
         <v>0</v>
       </c>
       <c r="F184">
-        <f>(D184-E184)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G184">
@@ -5892,14 +5892,14 @@
         <v>0</v>
       </c>
       <c r="D185">
-        <f>SUM(B185, C185)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E185">
         <v>0</v>
       </c>
       <c r="F185">
-        <f>(D185-E185)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G185">
@@ -5917,14 +5917,14 @@
         <v>0</v>
       </c>
       <c r="D186">
-        <f>SUM(B186, C186)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E186">
         <v>0</v>
       </c>
       <c r="F186">
-        <f>(D186-E186)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G186">
@@ -5942,14 +5942,14 @@
         <v>0</v>
       </c>
       <c r="D187">
-        <f>SUM(B187, C187)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E187">
         <v>0</v>
       </c>
       <c r="F187">
-        <f>(D187-E187)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G187">
@@ -5967,14 +5967,14 @@
         <v>0</v>
       </c>
       <c r="D188">
-        <f>SUM(B188, C188)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E188">
         <v>0</v>
       </c>
       <c r="F188">
-        <f>(D188-E188)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G188">
@@ -5992,14 +5992,14 @@
         <v>0</v>
       </c>
       <c r="D189">
-        <f>SUM(B189, C189)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E189">
         <v>0</v>
       </c>
       <c r="F189">
-        <f>(D189-E189)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G189">
@@ -6017,14 +6017,14 @@
         <v>0</v>
       </c>
       <c r="D190">
-        <f>SUM(B190, C190)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E190">
         <v>0</v>
       </c>
       <c r="F190">
-        <f>(D190-E190)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G190">
@@ -6042,14 +6042,14 @@
         <v>0</v>
       </c>
       <c r="D191">
-        <f>SUM(B191, C191)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E191">
         <v>0</v>
       </c>
       <c r="F191">
-        <f>(D191-E191)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G191">
@@ -6067,14 +6067,14 @@
         <v>0</v>
       </c>
       <c r="D192">
-        <f>SUM(B192, C192)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E192">
         <v>0</v>
       </c>
       <c r="F192">
-        <f>(D192-E192)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G192">
@@ -6092,14 +6092,14 @@
         <v>0</v>
       </c>
       <c r="D193">
-        <f>SUM(B193, C193)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E193">
         <v>0</v>
       </c>
       <c r="F193">
-        <f>(D193-E193)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G193">
@@ -6117,14 +6117,14 @@
         <v>0</v>
       </c>
       <c r="D194">
-        <f>SUM(B194, C194)</f>
+        <f t="shared" ref="D194:D257" si="6">SUM(B194, C194)</f>
         <v>0</v>
       </c>
       <c r="E194">
         <v>0</v>
       </c>
       <c r="F194">
-        <f>(D194-E194)</f>
+        <f t="shared" ref="F194:F257" si="7">(D194-E194)</f>
         <v>0</v>
       </c>
       <c r="G194" s="3">
@@ -6145,14 +6145,14 @@
         <v>0</v>
       </c>
       <c r="D195">
-        <f>SUM(B195, C195)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="E195">
         <v>0</v>
       </c>
       <c r="F195">
-        <f>(D195-E195)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G195">
@@ -6170,14 +6170,14 @@
         <v>0</v>
       </c>
       <c r="D196">
-        <f>SUM(B196, C196)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="E196">
         <v>0</v>
       </c>
       <c r="F196">
-        <f>(D196-E196)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G196">
@@ -6195,14 +6195,14 @@
         <v>0</v>
       </c>
       <c r="D197">
-        <f>SUM(B197, C197)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="E197">
         <v>0</v>
       </c>
       <c r="F197">
-        <f>(D197-E197)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G197">
@@ -6220,14 +6220,14 @@
         <v>0</v>
       </c>
       <c r="D198">
-        <f>SUM(B198, C198)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="E198">
         <v>0</v>
       </c>
       <c r="F198">
-        <f>(D198-E198)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G198">
@@ -6245,14 +6245,14 @@
         <v>0</v>
       </c>
       <c r="D199">
-        <f>SUM(B199, C199)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="E199">
         <v>0</v>
       </c>
       <c r="F199">
-        <f>(D199-E199)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G199">
@@ -6270,14 +6270,14 @@
         <v>0</v>
       </c>
       <c r="D200">
-        <f>SUM(B200, C200)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="E200">
         <v>0</v>
       </c>
       <c r="F200">
-        <f>(D200-E200)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G200">
@@ -6295,14 +6295,14 @@
         <v>0</v>
       </c>
       <c r="D201">
-        <f>SUM(B201, C201)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="E201">
         <v>0</v>
       </c>
       <c r="F201">
-        <f>(D201-E201)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G201">
@@ -6320,14 +6320,14 @@
         <v>0</v>
       </c>
       <c r="D202">
-        <f>SUM(B202, C202)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="E202">
         <v>0</v>
       </c>
       <c r="F202">
-        <f>(D202-E202)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G202">
@@ -6345,14 +6345,14 @@
         <v>0</v>
       </c>
       <c r="D203">
-        <f>SUM(B203, C203)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="E203">
         <v>0</v>
       </c>
       <c r="F203">
-        <f>(D203-E203)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G203">
@@ -6370,14 +6370,14 @@
         <v>0</v>
       </c>
       <c r="D204">
-        <f>SUM(B204, C204)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="E204">
         <v>0</v>
       </c>
       <c r="F204">
-        <f>(D204-E204)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G204">
@@ -6395,14 +6395,14 @@
         <v>0</v>
       </c>
       <c r="D205">
-        <f>SUM(B205, C205)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="E205">
         <v>0</v>
       </c>
       <c r="F205">
-        <f>(D205-E205)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G205">
@@ -6420,14 +6420,14 @@
         <v>0</v>
       </c>
       <c r="D206">
-        <f>SUM(B206, C206)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="E206">
         <v>0</v>
       </c>
       <c r="F206">
-        <f>(D206-E206)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G206">
@@ -6445,14 +6445,14 @@
         <v>0</v>
       </c>
       <c r="D207">
-        <f>SUM(B207, C207)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="E207">
         <v>0</v>
       </c>
       <c r="F207">
-        <f>(D207-E207)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G207">
@@ -6470,14 +6470,14 @@
         <v>0</v>
       </c>
       <c r="D208">
-        <f>SUM(B208, C208)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="E208">
         <v>0</v>
       </c>
       <c r="F208">
-        <f>(D208-E208)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G208">
@@ -6495,14 +6495,14 @@
         <v>0</v>
       </c>
       <c r="D209">
-        <f>SUM(B209, C209)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="E209">
         <v>0</v>
       </c>
       <c r="F209">
-        <f>(D209-E209)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G209">
@@ -6520,14 +6520,14 @@
         <v>0</v>
       </c>
       <c r="D210">
-        <f>SUM(B210, C210)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="E210">
         <v>0</v>
       </c>
       <c r="F210">
-        <f>(D210-E210)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G210">
@@ -6545,14 +6545,14 @@
         <v>0</v>
       </c>
       <c r="D211">
-        <f>SUM(B211, C211)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="E211">
         <v>0</v>
       </c>
       <c r="F211">
-        <f>(D211-E211)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G211">
@@ -6570,14 +6570,14 @@
         <v>0</v>
       </c>
       <c r="D212">
-        <f>SUM(B212, C212)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="E212">
         <v>0</v>
       </c>
       <c r="F212">
-        <f>(D212-E212)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G212">
@@ -6595,14 +6595,14 @@
         <v>0</v>
       </c>
       <c r="D213">
-        <f>SUM(B213, C213)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="E213">
         <v>0</v>
       </c>
       <c r="F213">
-        <f>(D213-E213)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G213">
@@ -6620,14 +6620,14 @@
         <v>0</v>
       </c>
       <c r="D214">
-        <f>SUM(B214, C214)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="E214">
         <v>0</v>
       </c>
       <c r="F214">
-        <f>(D214-E214)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G214">
@@ -6645,14 +6645,14 @@
         <v>0</v>
       </c>
       <c r="D215">
-        <f>SUM(B215, C215)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="E215">
         <v>0</v>
       </c>
       <c r="F215">
-        <f>(D215-E215)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G215">
@@ -6670,14 +6670,14 @@
         <v>0</v>
       </c>
       <c r="D216">
-        <f>SUM(B216, C216)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="E216">
         <v>0</v>
       </c>
       <c r="F216">
-        <f>(D216-E216)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G216">
@@ -6695,14 +6695,14 @@
         <v>0</v>
       </c>
       <c r="D217">
-        <f>SUM(B217, C217)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="E217">
         <v>0</v>
       </c>
       <c r="F217">
-        <f>(D217-E217)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G217">
@@ -6720,14 +6720,14 @@
         <v>0</v>
       </c>
       <c r="D218">
-        <f>SUM(B218, C218)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="E218">
         <v>0</v>
       </c>
       <c r="F218">
-        <f>(D218-E218)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G218">
@@ -6745,14 +6745,14 @@
         <v>0</v>
       </c>
       <c r="D219">
-        <f>SUM(B219, C219)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="E219">
         <v>0</v>
       </c>
       <c r="F219">
-        <f>(D219-E219)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G219">
@@ -6770,14 +6770,14 @@
         <v>0</v>
       </c>
       <c r="D220">
-        <f>SUM(B220, C220)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="E220">
         <v>0</v>
       </c>
       <c r="F220">
-        <f>(D220-E220)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G220">
@@ -6795,14 +6795,14 @@
         <v>0</v>
       </c>
       <c r="D221">
-        <f>SUM(B221, C221)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="E221">
         <v>0</v>
       </c>
       <c r="F221">
-        <f>(D221-E221)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G221">
@@ -6820,14 +6820,14 @@
         <v>0</v>
       </c>
       <c r="D222">
-        <f>SUM(B222, C222)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="E222">
         <v>0</v>
       </c>
       <c r="F222">
-        <f>(D222-E222)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G222">
@@ -6845,14 +6845,14 @@
         <v>0</v>
       </c>
       <c r="D223">
-        <f>SUM(B223, C223)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="E223">
         <v>0</v>
       </c>
       <c r="F223">
-        <f>(D223-E223)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G223">
@@ -6870,14 +6870,14 @@
         <v>0</v>
       </c>
       <c r="D224">
-        <f>SUM(B224, C224)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="E224">
         <v>0</v>
       </c>
       <c r="F224">
-        <f>(D224-E224)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G224">
@@ -6895,14 +6895,14 @@
         <v>0</v>
       </c>
       <c r="D225">
-        <f>SUM(B225, C225)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="E225">
         <v>0</v>
       </c>
       <c r="F225">
-        <f>(D225-E225)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G225">
@@ -6920,14 +6920,14 @@
         <v>0</v>
       </c>
       <c r="D226">
-        <f>SUM(B226, C226)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="E226">
         <v>0</v>
       </c>
       <c r="F226">
-        <f>(D226-E226)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G226">
@@ -6945,14 +6945,14 @@
         <v>0</v>
       </c>
       <c r="D227">
-        <f>SUM(B227, C227)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="E227">
         <v>0</v>
       </c>
       <c r="F227">
-        <f>(D227-E227)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G227">
@@ -6970,14 +6970,14 @@
         <v>0</v>
       </c>
       <c r="D228">
-        <f>SUM(B228, C228)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="E228">
         <v>0</v>
       </c>
       <c r="F228">
-        <f>(D228-E228)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G228">
@@ -6995,14 +6995,14 @@
         <v>0</v>
       </c>
       <c r="D229">
-        <f>SUM(B229, C229)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="E229">
         <v>0</v>
       </c>
       <c r="F229">
-        <f>(D229-E229)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G229">
@@ -7020,14 +7020,14 @@
         <v>0</v>
       </c>
       <c r="D230">
-        <f>SUM(B230, C230)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="E230">
         <v>0</v>
       </c>
       <c r="F230">
-        <f>(D230-E230)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G230">
@@ -7045,14 +7045,14 @@
         <v>0</v>
       </c>
       <c r="D231">
-        <f>SUM(B231, C231)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="E231">
         <v>0</v>
       </c>
       <c r="F231">
-        <f>(D231-E231)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G231">
@@ -7070,14 +7070,14 @@
         <v>0</v>
       </c>
       <c r="D232">
-        <f>SUM(B232, C232)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="E232">
         <v>0</v>
       </c>
       <c r="F232">
-        <f>(D232-E232)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G232">
@@ -7095,14 +7095,14 @@
         <v>0</v>
       </c>
       <c r="D233">
-        <f>SUM(B233, C233)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="E233">
         <v>0</v>
       </c>
       <c r="F233">
-        <f>(D233-E233)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G233">

</xml_diff>